<commit_message>
1. Updated spreadsheets atfer cmip5 initialisation error fix.
</commit_message>
<xml_diff>
--- a/cmip6/models/cnrm-cm6-1-hr/cmip6_cnrm-cerfacs_cnrm-cm6-1-hr_aerosol.xlsx
+++ b/cmip6/models/cnrm-cm6-1-hr/cmip6_cnrm-cerfacs_cnrm-cm6-1-hr_aerosol.xlsx
@@ -207,16 +207,16 @@
     <t>cmip6.aerosol.key_properties.scheme_scope</t>
   </si>
   <si>
-    <t>Troposphere</t>
-  </si>
-  <si>
-    <t>Stratosphere</t>
-  </si>
-  <si>
-    <t>Mesosphere</t>
-  </si>
-  <si>
-    <t>Whole atmosphere</t>
+    <t>troposphere</t>
+  </si>
+  <si>
+    <t>stratosphere</t>
+  </si>
+  <si>
+    <t>mesosphere</t>
+  </si>
+  <si>
+    <t>whole atmosphere</t>
   </si>
   <si>
     <t>Other: document in cell to the right</t>

</xml_diff>

<commit_message>
Revert "1. Updated spreadsheets atfer cmip5 initialisation error fix."
This reverts commit 35becf0596ac07b24f065152d6afb7f259330922.
</commit_message>
<xml_diff>
--- a/cmip6/models/cnrm-cm6-1-hr/cmip6_cnrm-cerfacs_cnrm-cm6-1-hr_aerosol.xlsx
+++ b/cmip6/models/cnrm-cm6-1-hr/cmip6_cnrm-cerfacs_cnrm-cm6-1-hr_aerosol.xlsx
@@ -207,16 +207,16 @@
     <t>cmip6.aerosol.key_properties.scheme_scope</t>
   </si>
   <si>
-    <t>troposphere</t>
-  </si>
-  <si>
-    <t>stratosphere</t>
-  </si>
-  <si>
-    <t>mesosphere</t>
-  </si>
-  <si>
-    <t>whole atmosphere</t>
+    <t>Troposphere</t>
+  </si>
+  <si>
+    <t>Stratosphere</t>
+  </si>
+  <si>
+    <t>Mesosphere</t>
+  </si>
+  <si>
+    <t>Whole atmosphere</t>
   </si>
   <si>
     <t>Other: document in cell to the right</t>

</xml_diff>